<commit_message>
feat: update BagMain UI
更新背包UI
</commit_message>
<xml_diff>
--- a/Excels/Npc_非玩家角色表.xlsx
+++ b/Excels/Npc_非玩家角色表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MetaApp\Editor_Win64\MetaWorldSaved\Saved\MetaWorld\Project\Edit\DragonVerse\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5137D57-A84C-4F1A-BEA6-F56BC115B77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82FB149-CEA2-415E-BF42-62F3ED085ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -483,7 +483,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.44140625" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -572,7 +572,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>18</v>

</xml_diff>